<commit_message>
4/20/2023: Redoing the regression only portion with new data.
</commit_message>
<xml_diff>
--- a/Positive Ki.xlsx
+++ b/Positive Ki.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sjsu0-my.sharepoint.com/personal/peter_v_pham_sjsu_edu/Documents/Antithrombin Feature Extraction/Regression/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="11_B7704AFEA7B4D302D6F20DB4C4A2D0A77AFFD4B6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3CDB90ED-DAF5-47A0-8DF9-408DAD7A9DFF}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="11_B7704AFEA7B4D302D6F20DB4C4A2D0A77AFFD4B6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AEAE501D-A6A3-4DB1-B938-F5E692883B64}"/>
   <bookViews>
-    <workbookView xWindow="4150" yWindow="3600" windowWidth="28800" windowHeight="15370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7000" yWindow="420" windowWidth="28800" windowHeight="15370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -275,11 +275,6 @@
     <t>infestin 1-2</t>
   </si>
   <si>
-    <t>LEENDCACPRVLHRVCGSDGNTYSNPCTLDCAKHEGKPDLVQVHEGP
-CDPNDHDFEDPECDNKFEPVCGTDHITYSNLCHLECAAFTTSPGVEVK
-YEGECHAE</t>
-  </si>
-  <si>
     <t>sp|Q8WPI2|16-142</t>
   </si>
   <si>
@@ -398,6 +393,9 @@
   </si>
   <si>
     <t>KI (nM)</t>
+  </si>
+  <si>
+    <t>LEENDCACPRVLHRVCGSDGNTYSNPCTLDCAKHEGKPDLVQVHEGPCDPNDHDFEDPECDNKFEPVCGTDHITYSNLCHLECAAFTTSPGVEVKYEGECHAE</t>
   </si>
 </sst>
 </file>
@@ -744,7 +742,7 @@
   <dimension ref="A1:D1000"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="C44" sqref="C44"/>
+      <selection activeCell="I43" sqref="I43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1"/>
@@ -765,7 +763,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15.75" customHeight="1">
@@ -1384,16 +1382,16 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="72.5">
+    <row r="44" spans="1:4" ht="43.5">
       <c r="A44" s="3" t="s">
         <v>78</v>
       </c>
       <c r="B44" s="3">
         <f t="shared" si="0"/>
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>79</v>
+        <v>119</v>
       </c>
       <c r="D44" s="8">
         <v>2.5000000000000001E-2</v>
@@ -1401,14 +1399,14 @@
     </row>
     <row r="45" spans="1:4" ht="58">
       <c r="A45" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B45" s="3">
+        <f t="shared" si="0"/>
+        <v>127</v>
+      </c>
+      <c r="C45" s="3" t="s">
         <v>80</v>
-      </c>
-      <c r="B45" s="3">
-        <f t="shared" si="0"/>
-        <v>127</v>
-      </c>
-      <c r="C45" s="3" t="s">
-        <v>81</v>
       </c>
       <c r="D45" s="4">
         <v>1.8</v>
@@ -1416,27 +1414,27 @@
     </row>
     <row r="46" spans="1:4" ht="29">
       <c r="A46" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B46" s="3">
+        <f t="shared" si="0"/>
+        <v>55</v>
+      </c>
+      <c r="C46" s="3" t="s">
         <v>82</v>
-      </c>
-      <c r="B46" s="3">
-        <f t="shared" si="0"/>
-        <v>55</v>
-      </c>
-      <c r="C46" s="3" t="s">
-        <v>83</v>
       </c>
       <c r="D46" s="4"/>
     </row>
     <row r="47" spans="1:4" ht="116">
       <c r="A47" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B47" s="3">
+        <f t="shared" si="0"/>
+        <v>259</v>
+      </c>
+      <c r="C47" s="3" t="s">
         <v>84</v>
-      </c>
-      <c r="B47" s="3">
-        <f t="shared" si="0"/>
-        <v>259</v>
-      </c>
-      <c r="C47" s="3" t="s">
-        <v>85</v>
       </c>
       <c r="D47" s="4">
         <v>30</v>
@@ -1449,7 +1447,7 @@
         <v>4</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D48" s="4">
         <v>17.2</v>
@@ -1457,14 +1455,14 @@
     </row>
     <row r="49" spans="1:4" ht="72.5">
       <c r="A49" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B49" s="3">
+        <f t="shared" si="0"/>
+        <v>152</v>
+      </c>
+      <c r="C49" s="3" t="s">
         <v>87</v>
-      </c>
-      <c r="B49" s="3">
-        <f t="shared" si="0"/>
-        <v>152</v>
-      </c>
-      <c r="C49" s="3" t="s">
-        <v>88</v>
       </c>
       <c r="D49" s="4">
         <v>20</v>
@@ -1472,14 +1470,14 @@
     </row>
     <row r="50" spans="1:4" ht="14.5">
       <c r="A50" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B50" s="3">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="C50" s="3" t="s">
         <v>89</v>
-      </c>
-      <c r="B50" s="3">
-        <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="C50" s="3" t="s">
-        <v>90</v>
       </c>
       <c r="D50" s="4">
         <v>29</v>
@@ -1487,14 +1485,14 @@
     </row>
     <row r="51" spans="1:4" ht="29">
       <c r="A51" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B51" s="3">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+      <c r="C51" s="3" t="s">
         <v>91</v>
-      </c>
-      <c r="B51" s="3">
-        <f t="shared" si="0"/>
-        <v>60</v>
-      </c>
-      <c r="C51" s="3" t="s">
-        <v>92</v>
       </c>
       <c r="D51" s="4">
         <v>55.6</v>
@@ -1502,14 +1500,14 @@
     </row>
     <row r="52" spans="1:4" ht="29">
       <c r="A52" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B52" s="3">
+        <f t="shared" si="0"/>
+        <v>70</v>
+      </c>
+      <c r="C52" s="3" t="s">
         <v>93</v>
-      </c>
-      <c r="B52" s="3">
-        <f t="shared" si="0"/>
-        <v>70</v>
-      </c>
-      <c r="C52" s="3" t="s">
-        <v>94</v>
       </c>
       <c r="D52" s="4">
         <v>214.4</v>
@@ -1517,14 +1515,14 @@
     </row>
     <row r="53" spans="1:4" ht="29">
       <c r="A53" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B53" s="3">
+        <f t="shared" si="0"/>
+        <v>65</v>
+      </c>
+      <c r="C53" s="3" t="s">
         <v>95</v>
-      </c>
-      <c r="B53" s="3">
-        <f t="shared" si="0"/>
-        <v>65</v>
-      </c>
-      <c r="C53" s="3" t="s">
-        <v>96</v>
       </c>
       <c r="D53" s="9">
         <v>320</v>
@@ -1532,14 +1530,14 @@
     </row>
     <row r="54" spans="1:4" ht="29">
       <c r="A54" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B54" s="3">
+        <f t="shared" si="0"/>
+        <v>54</v>
+      </c>
+      <c r="C54" s="3" t="s">
         <v>97</v>
-      </c>
-      <c r="B54" s="3">
-        <f t="shared" si="0"/>
-        <v>54</v>
-      </c>
-      <c r="C54" s="3" t="s">
-        <v>98</v>
       </c>
       <c r="D54" s="9">
         <v>26000</v>
@@ -1547,14 +1545,14 @@
     </row>
     <row r="55" spans="1:4" ht="29">
       <c r="A55" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="B55" s="3">
+        <f t="shared" si="0"/>
+        <v>59</v>
+      </c>
+      <c r="C55" s="3" t="s">
         <v>99</v>
-      </c>
-      <c r="B55" s="3">
-        <f t="shared" si="0"/>
-        <v>59</v>
-      </c>
-      <c r="C55" s="3" t="s">
-        <v>100</v>
       </c>
       <c r="D55" s="4">
         <v>290</v>
@@ -1562,14 +1560,14 @@
     </row>
     <row r="56" spans="1:4" ht="29">
       <c r="A56" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="B56" s="3">
+        <f t="shared" si="0"/>
+        <v>59</v>
+      </c>
+      <c r="C56" s="3" t="s">
         <v>101</v>
-      </c>
-      <c r="B56" s="3">
-        <f t="shared" si="0"/>
-        <v>59</v>
-      </c>
-      <c r="C56" s="3" t="s">
-        <v>102</v>
       </c>
       <c r="D56" s="4">
         <v>210</v>
@@ -1577,14 +1575,14 @@
     </row>
     <row r="57" spans="1:4" ht="14.5">
       <c r="A57" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="B57" s="3">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="C57" s="3" t="s">
         <v>103</v>
-      </c>
-      <c r="B57" s="3">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="C57" s="3" t="s">
-        <v>104</v>
       </c>
       <c r="D57" s="4">
         <v>61000</v>
@@ -1592,14 +1590,14 @@
     </row>
     <row r="58" spans="1:4" ht="29">
       <c r="A58" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="B58" s="3">
+        <f t="shared" si="0"/>
+        <v>63</v>
+      </c>
+      <c r="C58" s="3" t="s">
         <v>105</v>
-      </c>
-      <c r="B58" s="3">
-        <f t="shared" si="0"/>
-        <v>63</v>
-      </c>
-      <c r="C58" s="3" t="s">
-        <v>106</v>
       </c>
       <c r="D58" s="4">
         <v>5.8E-5</v>
@@ -1607,14 +1605,14 @@
     </row>
     <row r="59" spans="1:4" ht="29">
       <c r="A59" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B59" s="3">
+        <f t="shared" si="0"/>
+        <v>69</v>
+      </c>
+      <c r="C59" s="3" t="s">
         <v>107</v>
-      </c>
-      <c r="B59" s="3">
-        <f t="shared" si="0"/>
-        <v>69</v>
-      </c>
-      <c r="C59" s="3" t="s">
-        <v>108</v>
       </c>
       <c r="D59" s="8">
         <v>2970</v>
@@ -1622,14 +1620,14 @@
     </row>
     <row r="60" spans="1:4" ht="87">
       <c r="A60" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="B60" s="3">
+        <f t="shared" si="0"/>
+        <v>187</v>
+      </c>
+      <c r="C60" s="3" t="s">
         <v>109</v>
-      </c>
-      <c r="B60" s="3">
-        <f t="shared" si="0"/>
-        <v>187</v>
-      </c>
-      <c r="C60" s="3" t="s">
-        <v>110</v>
       </c>
       <c r="D60" s="7">
         <v>380</v>
@@ -1637,7 +1635,7 @@
     </row>
     <row r="61" spans="1:4" ht="14.5">
       <c r="A61" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B61" s="3">
         <f t="shared" si="0"/>
@@ -1657,7 +1655,7 @@
         <v>18</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D62" s="4">
         <v>64.5</v>
@@ -1665,14 +1663,14 @@
     </row>
     <row r="63" spans="1:4" ht="29">
       <c r="A63" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B63" s="3">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="C63" s="3" t="s">
         <v>113</v>
-      </c>
-      <c r="B63" s="3">
-        <f t="shared" si="0"/>
-        <v>40</v>
-      </c>
-      <c r="C63" s="3" t="s">
-        <v>114</v>
       </c>
       <c r="D63" s="7">
         <v>4000</v>
@@ -1680,14 +1678,14 @@
     </row>
     <row r="64" spans="1:4" ht="29">
       <c r="A64" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="B64" s="3">
+        <f t="shared" si="0"/>
+        <v>65</v>
+      </c>
+      <c r="C64" s="3" t="s">
         <v>115</v>
-      </c>
-      <c r="B64" s="3">
-        <f t="shared" si="0"/>
-        <v>65</v>
-      </c>
-      <c r="C64" s="3" t="s">
-        <v>116</v>
       </c>
       <c r="D64" s="4">
         <v>6.0000000000000002E-5</v>
@@ -1695,14 +1693,14 @@
     </row>
     <row r="65" spans="1:4" ht="14.5">
       <c r="A65" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="B65" s="3">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="C65" s="3" t="s">
         <v>117</v>
-      </c>
-      <c r="B65" s="3">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="C65" s="3" t="s">
-        <v>118</v>
       </c>
       <c r="D65" s="9">
         <v>1750000</v>

</xml_diff>

<commit_message>
4/30/2023: Cleaned new data.
</commit_message>
<xml_diff>
--- a/Positive Ki.xlsx
+++ b/Positive Ki.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sjsu0-my.sharepoint.com/personal/peter_v_pham_sjsu_edu/Documents/Antithrombin Feature Extraction/Regression/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="11_B7704AFEA7B4D302D6F20DB4C4A2D0A77AFFD4B6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AEAE501D-A6A3-4DB1-B938-F5E692883B64}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="11_B7704AFEA7B4D302D6F20DB4C4A2D0A77AFFD4B6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0C3A7DD6-2BF4-437F-B396-075A1FA51877}"/>
   <bookViews>
     <workbookView xWindow="7000" yWindow="420" windowWidth="28800" windowHeight="15370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -532,10 +532,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -742,7 +738,7 @@
   <dimension ref="A1:D1000"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="I43" sqref="I43"/>
+      <selection activeCell="D47" sqref="D47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1"/>
@@ -1423,7 +1419,9 @@
       <c r="C46" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="D46" s="4"/>
+      <c r="D46" s="4">
+        <v>7.5</v>
+      </c>
     </row>
     <row r="47" spans="1:4" ht="116">
       <c r="A47" s="3" t="s">

</xml_diff>